<commit_message>
All fixed. Experiment 1 finished
</commit_message>
<xml_diff>
--- a/Experiment 1/Trace Files/ThroughputGraph.xlsx
+++ b/Experiment 1/Trace Files/ThroughputGraph.xlsx
@@ -241,34 +241,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>7.7754468604099998</c:v>
+                  <c:v>436.615583082</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8.7637969466300003</c:v>
+                  <c:v>457.337711974</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9.7521470328500008</c:v>
+                  <c:v>475.31725117600001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10.7404971191</c:v>
+                  <c:v>490.58223224099999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>11.728847205299999</c:v>
+                  <c:v>504.01554340500002</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>12.4455734533</c:v>
+                  <c:v>517.23549521899997</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>13.372040653000001</c:v>
+                  <c:v>523.99744624699997</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>11.9899556247</c:v>
+                  <c:v>512.83996144499997</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>11.294376918899999</c:v>
+                  <c:v>551.12267764800004</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>9.9845175996699993</c:v>
+                  <c:v>466.18050928000002</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -347,34 +347,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>7.7754468604099998</c:v>
+                  <c:v>436.615583082</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8.7637969466300003</c:v>
+                  <c:v>457.337711974</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9.7521470328500008</c:v>
+                  <c:v>475.31725117600001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10.7404971191</c:v>
+                  <c:v>490.58223224099999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>11.728847205299999</c:v>
+                  <c:v>504.01554340500002</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>11.979543256099999</c:v>
+                  <c:v>522.65243003600006</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>12.933210945500001</c:v>
+                  <c:v>529.01848125399999</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>10.895236492900001</c:v>
+                  <c:v>554.62067992100003</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>10.577347857199999</c:v>
+                  <c:v>583.84376187199996</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>9.9863667921299992</c:v>
+                  <c:v>465.865871314</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -453,34 +453,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>7.7754468604099998</c:v>
+                  <c:v>436.615583082</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8.7637969466300003</c:v>
+                  <c:v>457.337711974</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9.7521470328500008</c:v>
+                  <c:v>475.31725117600001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10.7404971191</c:v>
+                  <c:v>490.58223224099999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>11.728847205299999</c:v>
+                  <c:v>504.01554340500002</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>12.3692644152</c:v>
+                  <c:v>518.277151581</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>13.320253296200001</c:v>
+                  <c:v>524.46795580699995</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>11.9669057183</c:v>
+                  <c:v>510.59175602400001</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>11.0149472179</c:v>
+                  <c:v>560.42559472300002</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>10.089414043</c:v>
+                  <c:v>465.28300623000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -559,34 +559,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>7.4031879547499999</c:v>
+                  <c:v>423.87633241600003</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8.3915380409600004</c:v>
+                  <c:v>445.37962413299999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9.3798881271799992</c:v>
+                  <c:v>464.46806234100001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10.3682382134</c:v>
+                  <c:v>480.91494584600002</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>11.213088278600001</c:v>
+                  <c:v>496.56164433200001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>12.0404087984</c:v>
+                  <c:v>509.27854533499999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>13.1653286759</c:v>
+                  <c:v>512.28365244199995</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>13.094264863599999</c:v>
+                  <c:v>441.28550654700001</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>11.830693527399999</c:v>
+                  <c:v>463.23658880800002</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>9.9139146879600002</c:v>
+                  <c:v>465.03944311999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -602,11 +602,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-188291744"/>
-        <c:axId val="-188290112"/>
+        <c:axId val="1153167072"/>
+        <c:axId val="1153160000"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-188291744"/>
+        <c:axId val="1153167072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -705,7 +705,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-188290112"/>
+        <c:crossAx val="1153160000"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -713,10 +713,10 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-188290112"/>
+        <c:axId val="1153160000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:min val="6"/>
+          <c:min val="400"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -755,7 +755,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Throughput (Mbps)</a:t>
+                  <a:t>Throughput (Kbps)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -821,7 +821,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-188291744"/>
+        <c:crossAx val="1153167072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1759,7 +1759,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M21" sqref="M21"/>
+      <selection activeCell="E2" sqref="E2:E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.55" x14ac:dyDescent="0.3"/>
@@ -1786,16 +1786,16 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>7.7754468604099998</v>
+        <v>436.615583082</v>
       </c>
       <c r="C2">
-        <v>7.7754468604099998</v>
+        <v>436.615583082</v>
       </c>
       <c r="D2">
-        <v>7.7754468604099998</v>
+        <v>436.615583082</v>
       </c>
       <c r="E2">
-        <v>7.4031879547499999</v>
+        <v>423.87633241600003</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -1803,16 +1803,16 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>8.7637969466300003</v>
+        <v>457.337711974</v>
       </c>
       <c r="C3">
-        <v>8.7637969466300003</v>
+        <v>457.337711974</v>
       </c>
       <c r="D3">
-        <v>8.7637969466300003</v>
+        <v>457.337711974</v>
       </c>
       <c r="E3">
-        <v>8.3915380409600004</v>
+        <v>445.37962413299999</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -1820,16 +1820,16 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>9.7521470328500008</v>
+        <v>475.31725117600001</v>
       </c>
       <c r="C4">
-        <v>9.7521470328500008</v>
+        <v>475.31725117600001</v>
       </c>
       <c r="D4">
-        <v>9.7521470328500008</v>
+        <v>475.31725117600001</v>
       </c>
       <c r="E4">
-        <v>9.3798881271799992</v>
+        <v>464.46806234100001</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -1837,16 +1837,16 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>10.7404971191</v>
+        <v>490.58223224099999</v>
       </c>
       <c r="C5">
-        <v>10.7404971191</v>
+        <v>490.58223224099999</v>
       </c>
       <c r="D5">
-        <v>10.7404971191</v>
+        <v>490.58223224099999</v>
       </c>
       <c r="E5">
-        <v>10.3682382134</v>
+        <v>480.91494584600002</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -1854,16 +1854,16 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>11.728847205299999</v>
+        <v>504.01554340500002</v>
       </c>
       <c r="C6">
-        <v>11.728847205299999</v>
+        <v>504.01554340500002</v>
       </c>
       <c r="D6">
-        <v>11.728847205299999</v>
+        <v>504.01554340500002</v>
       </c>
       <c r="E6">
-        <v>11.213088278600001</v>
+        <v>496.56164433200001</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -1871,16 +1871,16 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>12.4455734533</v>
+        <v>517.23549521899997</v>
       </c>
       <c r="C7">
-        <v>11.979543256099999</v>
+        <v>522.65243003600006</v>
       </c>
       <c r="D7">
-        <v>12.3692644152</v>
+        <v>518.277151581</v>
       </c>
       <c r="E7">
-        <v>12.0404087984</v>
+        <v>509.27854533499999</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -1888,16 +1888,16 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>13.372040653000001</v>
+        <v>523.99744624699997</v>
       </c>
       <c r="C8">
-        <v>12.933210945500001</v>
+        <v>529.01848125399999</v>
       </c>
       <c r="D8">
-        <v>13.320253296200001</v>
+        <v>524.46795580699995</v>
       </c>
       <c r="E8">
-        <v>13.1653286759</v>
+        <v>512.28365244199995</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -1905,16 +1905,16 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>11.9899556247</v>
+        <v>512.83996144499997</v>
       </c>
       <c r="C9">
-        <v>10.895236492900001</v>
+        <v>554.62067992100003</v>
       </c>
       <c r="D9">
-        <v>11.9669057183</v>
+        <v>510.59175602400001</v>
       </c>
       <c r="E9">
-        <v>13.094264863599999</v>
+        <v>441.28550654700001</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
@@ -1922,16 +1922,16 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>11.294376918899999</v>
+        <v>551.12267764800004</v>
       </c>
       <c r="C10">
-        <v>10.577347857199999</v>
+        <v>583.84376187199996</v>
       </c>
       <c r="D10">
-        <v>11.0149472179</v>
+        <v>560.42559472300002</v>
       </c>
       <c r="E10">
-        <v>11.830693527399999</v>
+        <v>463.23658880800002</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
@@ -1939,16 +1939,16 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>9.9845175996699993</v>
+        <v>466.18050928000002</v>
       </c>
       <c r="C11">
-        <v>9.9863667921299992</v>
+        <v>465.865871314</v>
       </c>
       <c r="D11">
-        <v>10.089414043</v>
+        <v>465.28300623000001</v>
       </c>
       <c r="E11">
-        <v>9.9139146879600002</v>
+        <v>465.03944311999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>